<commit_message>
Commit at 1 Sept,2023 2:23AM
</commit_message>
<xml_diff>
--- a/hudi_work_done.xlsx
+++ b/hudi_work_done.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshumanr/Documents/Hudi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56214D93-FD7F-224B-9CD1-D1E97A54DAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D3FE75-0F0A-4142-90FC-0AF9773FE401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{1FDDDF64-3A77-BC4E-9A2F-B2FFE421C5EC}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16100" xr2:uid="{1FDDDF64-3A77-BC4E-9A2F-B2FFE421C5EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>TOPICS</t>
   </si>
@@ -84,13 +84,31 @@
   <si>
     <t>Timestamp format of Hudi table :                        YYYYMMDDhhmmssSSS                                          for example : 20230831160421605 means
 The year is 2023, the month is August, the day is 31, the hour is 16, the minute is 04, the second is 21, and the milliseconds are 605.</t>
+  </si>
+  <si>
+    <t>Creating a Partitioned table</t>
+  </si>
+  <si>
+    <t>Hudi Properties to Remember</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'hoodie.datasource.write.operation': 'upsert' or 'insert' or 'bulkinsert'. Use bulkinsert to load new data into a table, and there on use upsert/insert. bulk insert uses a disk based write path to scale to load large inputs without need to cache it.</t>
+  </si>
+  <si>
+    <t>Created table (accounts_non_partition) contains parquet files. Original file size : 62.3 MB            Hudi table size : 122.4 MB</t>
+  </si>
+  <si>
+    <t>Created table (accounts_partition which has) partitioned folders which contains parquet files. Original file size : 62.3 MB            Hudi table size : 123.4 MB</t>
+  </si>
+  <si>
+    <t>By default , hudi creates COW tables and the meta data files of those table are stored as a MOR table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +141,11 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -140,20 +163,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -166,17 +235,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,197 +597,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E456AC-905B-5A46-B6DE-A04D387217E8}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.1640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="53.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="43.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="49.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="53.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="43.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" style="6" customWidth="1"/>
     <col min="5" max="5" width="44.33203125" customWidth="1"/>
+    <col min="7" max="7" width="67.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="184" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="184" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="6" t="s">
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="100" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6" t="s">
+      <c r="G3" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="100" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="140" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="G4" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="10"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="4"/>
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="2"/>
     </row>
+    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="14"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="14"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="14"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="14"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="14"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="14"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="14"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="14"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="14"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="14"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="14"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="14"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B5"/>
+  <mergeCells count="10">
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="A2:A8"/>
     <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>